<commit_message>
make attendance func to be  like figma
</commit_message>
<xml_diff>
--- a/public/uploads/studentlist_261361.xlsx
+++ b/public/uploads/studentlist_261361.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMU\Y3\T2\SE_Project\project_se_t12\public\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMU\Y3\T2\SE_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA3F65A-254F-4F7B-997A-611E6553FD4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23439415-6090-4B39-835C-CA0B50D3D559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>รายชื่อนักศึกษาที่ลงทะเบียนเรียน ภาคเรียนที่ 2 ปีการศึกษา 2567</t>
   </si>
@@ -72,12 +72,18 @@
   <si>
     <t>พรรณเชษฐ์</t>
   </si>
+  <si>
+    <t>kittiwin_phannachet@cmu.ac.th</t>
+  </si>
+  <si>
+    <t>korarit@cmu.ac.th</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -102,6 +108,12 @@
       <color rgb="FF000000"/>
       <name val="Angsana New"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -171,10 +183,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -197,6 +210,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -208,11 +225,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -520,8 +535,8 @@
   </sheetPr>
   <dimension ref="A1:J122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,25 +545,26 @@
     <col min="2" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="6" width="25" customWidth="1"/>
+    <col min="9" max="9" width="29.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="26.4" x14ac:dyDescent="0.7">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="13"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="26.4" x14ac:dyDescent="0.7">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="3">
         <v>261361</v>
       </c>
@@ -565,14 +581,14 @@
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="26.4" x14ac:dyDescent="0.7">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="1"/>
@@ -591,10 +607,10 @@
       <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="14"/>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:10" ht="25.8" x14ac:dyDescent="0.65">
       <c r="A5" s="7">
@@ -603,7 +619,7 @@
       <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="7">
@@ -617,6 +633,9 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
+      <c r="I5" s="11" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="25.8" x14ac:dyDescent="0.65">
       <c r="A6" s="7"/>
@@ -729,6 +748,9 @@
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
+      <c r="I15" s="11" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="25.8" x14ac:dyDescent="0.65">
       <c r="A16" s="7"/>
@@ -1809,6 +1831,10 @@
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="E4:F4"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="I5" r:id="rId1" xr:uid="{E6221E8B-E9A9-47A7-B9E8-8EED58B20311}"/>
+    <hyperlink ref="I15" r:id="rId2" xr:uid="{C8973A0E-11B5-4922-BA10-7EF49A12C69B}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait"/>
 </worksheet>

</xml_diff>